<commit_message>
Se han añadido nuevos inputs y modificación restricción soft 2
</commit_message>
<xml_diff>
--- a/datos/Generador inputs horarios 1.xlsx
+++ b/datos/Generador inputs horarios 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2022C33E-B67F-4246-A364-6E08593EEBF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7008B9D3-27BB-401F-9F39-142C24D6D537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
       </c>
       <c r="E7">
         <f>SUM(D53:H53)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" t="str">
         <f>IF(E7&gt;=D7,"OK","ERROR")</f>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="L7" cm="1">
         <f t="array" ref="L7">IF(K7="","",INDEX($D$38:$AC$38,(ROW(K7)-ROW($K$7))*2+1))</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>22</v>
@@ -1032,11 +1032,11 @@
       </c>
       <c r="D8">
         <f>IF(C8="","",A40)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <f>SUM(D54:H54)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" ref="F8:F19" si="2">IF(E8&gt;=D8,"OK","ERROR")</f>
@@ -1070,11 +1070,11 @@
       </c>
       <c r="D9">
         <f>IF(C9="","",A41)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <f>SUM(D55:H55)</f>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="L9" s="18">
         <f>IF(K9="","",INDEX($D$38:$AC$38,(ROW(K9)-ROW($K$7))*2+1))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="E10">
         <f>SUM(D56:H56)</f>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E17" si="3">SUM(D57:H57)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="L11" cm="1">
         <f t="array" ref="L11">IF(K11="","",INDEX($D$38:$AC$38,(ROW(K11)-ROW($K$7))*2+1))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.25">
@@ -1157,11 +1157,11 @@
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D19" si="4">IF(C12="","",A44)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="L13" cm="1">
         <f t="array" ref="L13">IF(K13="","",INDEX($D$38:$AC$38,(ROW(K13)-ROW($K$7))*2+1))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -1273,11 +1273,11 @@
       </c>
       <c r="D16">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="L17" cm="1">
         <f t="array" ref="L17">IF(K17="","",INDEX($D$38:$AC$38,(ROW(K17)-ROW($K$7))*2+1))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>2</v>
@@ -1546,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="L24" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="21" t="s">
         <v>3</v>
@@ -1619,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>44</v>
       </c>
       <c r="X25" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y25" s="15" t="s">
         <v>45</v>
@@ -1704,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>1</v>
@@ -1728,7 +1728,7 @@
         <v>40</v>
       </c>
       <c r="P26" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="22" t="s">
         <v>41</v>
@@ -1777,7 +1777,7 @@
         <v>Clase D</v>
       </c>
       <c r="D27" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>0</v>
@@ -1789,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="22" t="s">
         <v>3</v>
@@ -2184,7 +2184,7 @@
     <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="D38">
         <f>SUM(D24:D28)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38">
         <f>SUM(E24:E27)</f>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="H38" s="19">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <f t="shared" si="7"/>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="L38">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M38">
         <f t="shared" si="7"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="P38">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q38">
         <f t="shared" si="7"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="X38">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y38">
         <f t="shared" si="7"/>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="D39" s="9">
         <f>SUMIFS(D$24:D$27,E$24:E$27,$C39)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" s="9">
         <f t="shared" ref="E39:AC39" si="8">SUMIFS(E$24:E$27,F$24:F$27,$C39)</f>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="H39" s="9">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="8"/>
@@ -2404,7 +2404,7 @@
     <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ref="A40:A51" si="9">SUM(C40:AB40)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="10" t="str">
         <f t="shared" ref="C40:C51" si="10">C8</f>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H40" s="10">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="10">
         <f t="shared" si="11"/>
@@ -2518,7 +2518,7 @@
     <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" s="10" t="str">
         <f t="shared" si="10"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="H41" s="10">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="10">
         <f t="shared" si="12"/>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="H42" s="10">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="10">
         <f t="shared" si="13"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="L42" s="10">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M42" s="10">
         <f t="shared" si="13"/>
@@ -2860,7 +2860,7 @@
     <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C44" s="10" t="str">
         <f t="shared" si="10"/>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="P44" s="10">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q44" s="10">
         <f t="shared" si="15"/>
@@ -3316,7 +3316,7 @@
     <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" s="10" t="str">
         <f t="shared" si="10"/>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="X48" s="10">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y48" s="10">
         <f t="shared" si="19"/>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="H53" s="30">
         <f t="shared" si="23"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="H54" s="28">
         <f t="shared" si="25"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="D55" s="28">
         <f>IF(D74="",D$90-D$89,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E55" s="28">
         <f t="shared" ref="E55:H55" si="26">IF(E74="",E$90-E$89,0)</f>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="H55" s="28">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="E56" s="28">
         <f t="shared" ref="E56:H56" si="27">IF(E75="",E$90-E$89,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F56" s="28">
         <f t="shared" si="27"/>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="H56" s="28">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="H57" s="28">
         <f t="shared" si="28"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="H58" s="28">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="10"/>
@@ -4087,15 +4087,15 @@
       </c>
       <c r="D59" s="28">
         <f t="shared" ref="D59:H59" si="30">IF(D78="",D$90-D$89,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E59" s="28">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F59" s="28">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G59" s="28">
         <f t="shared" si="30"/>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="H59" s="28">
         <f t="shared" si="30"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="H60" s="28">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="10"/>
@@ -4193,11 +4193,11 @@
       </c>
       <c r="G61" s="28">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H61" s="28">
         <f t="shared" si="32"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="10"/>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="H62" s="28">
         <f t="shared" si="33"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I62" s="10"/>
       <c r="J62" s="10"/>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="E63" s="28">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F63" s="28">
         <f t="shared" si="34"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="H63" s="28">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I63" s="10"/>
       <c r="J63" s="10"/>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="H64" s="28">
         <f t="shared" si="35"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I64" s="10"/>
       <c r="J64" s="10"/>
@@ -4385,7 +4385,7 @@
       </c>
       <c r="H65" s="27">
         <f t="shared" si="36"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
@@ -4586,9 +4586,7 @@
         <f t="shared" si="37"/>
         <v>MARIO</v>
       </c>
-      <c r="D74" s="15">
-        <v>1</v>
-      </c>
+      <c r="D74" s="15"/>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
@@ -4604,14 +4602,10 @@
         <v>MARIA</v>
       </c>
       <c r="D75" s="15"/>
-      <c r="E75" s="15">
-        <v>1</v>
-      </c>
+      <c r="E75" s="15"/>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="15">
-        <v>1</v>
-      </c>
+      <c r="H75" s="15"/>
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -4652,15 +4646,9 @@
         <f t="shared" si="37"/>
         <v>ANTONIA</v>
       </c>
-      <c r="D78" s="22">
-        <v>1</v>
-      </c>
-      <c r="E78" s="22">
-        <v>1</v>
-      </c>
-      <c r="F78" s="22">
-        <v>1</v>
-      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
       <c r="G78" s="22"/>
       <c r="H78" s="22"/>
     </row>
@@ -4691,9 +4679,7 @@
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
-      <c r="G80" s="22">
-        <v>1</v>
-      </c>
+      <c r="G80" s="22"/>
       <c r="H80" s="22"/>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
@@ -4721,9 +4707,7 @@
         <v>LAURA</v>
       </c>
       <c r="D82" s="22"/>
-      <c r="E82" s="22">
-        <v>1</v>
-      </c>
+      <c r="E82" s="22"/>
       <c r="F82" s="22"/>
       <c r="G82" s="22"/>
       <c r="H82" s="22"/>
@@ -4844,7 +4828,7 @@
         <v>14</v>
       </c>
       <c r="H90" s="24">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.25">
@@ -4853,7 +4837,7 @@
       </c>
       <c r="D92" s="25">
         <f>SUM(D90:H90)-SUM(D89:H89)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5020,7 +5004,7 @@
       </c>
       <c r="F2">
         <f>Sheet1!H24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="str">
         <f>Sheet1!I24</f>
@@ -5036,7 +5020,7 @@
       </c>
       <c r="J2">
         <f>Sheet1!L24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="str">
         <f>Sheet1!M24</f>
@@ -5130,7 +5114,7 @@
       </c>
       <c r="F3">
         <f>Sheet1!H25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="str">
         <f>Sheet1!I25</f>
@@ -5194,7 +5178,7 @@
       </c>
       <c r="V3">
         <f>Sheet1!X25</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W3" t="str">
         <f>Sheet1!Y25</f>
@@ -5240,7 +5224,7 @@
       </c>
       <c r="F4">
         <f>Sheet1!H26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="str">
         <f>Sheet1!I26</f>
@@ -5272,7 +5256,7 @@
       </c>
       <c r="N4">
         <f>Sheet1!P26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" t="str">
         <f>Sheet1!Q26</f>
@@ -5334,7 +5318,7 @@
       </c>
       <c r="B5">
         <f>Sheet1!D27</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="str">
         <f>Sheet1!E27</f>
@@ -5350,7 +5334,7 @@
       </c>
       <c r="F5">
         <f>Sheet1!H27</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="str">
         <f>Sheet1!I27</f>
@@ -6523,7 +6507,7 @@
       </c>
       <c r="B4">
         <f>Sheet1!D74</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>Sheet1!E74</f>
@@ -6553,7 +6537,7 @@
       </c>
       <c r="C5">
         <f>Sheet1!E75</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>Sheet1!F75</f>
@@ -6565,7 +6549,7 @@
       </c>
       <c r="F5">
         <f>Sheet1!H75</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6627,15 +6611,15 @@
       </c>
       <c r="B8">
         <f>Sheet1!D78</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>Sheet1!E78</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>Sheet1!F78</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f>Sheet1!G78</f>
@@ -6691,7 +6675,7 @@
       </c>
       <c r="E10">
         <f>Sheet1!G80</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f>Sheet1!H80</f>
@@ -6735,7 +6719,7 @@
       </c>
       <c r="C12">
         <f>Sheet1!E82</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f>Sheet1!F82</f>
@@ -6880,7 +6864,7 @@
       </c>
       <c r="E3">
         <f>Sheet1!H90</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>